<commit_message>
Update of the spreadsheets
</commit_message>
<xml_diff>
--- a/SWPattern/experimentalResults/LUBMDatasets/UniversityOtherOtherSets.xlsx
+++ b/SWPattern/experimentalResults/LUBMDatasets/UniversityOtherOtherSets.xlsx
@@ -5,25 +5,26 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datos\workingDir\krimp\3rdResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datos\git\SWKrimpSim\SWPattern\experimentalResults\LUBMDatasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="UniversityOtherOtherSets-Matrix" sheetId="2" r:id="rId1"/>
-    <sheet name="UniversityOtherOtherSets" sheetId="1" r:id="rId2"/>
+    <sheet name="LUBMSetsNoCTOtherSet-Matrix" sheetId="4" r:id="rId1"/>
+    <sheet name="LUBMSets-CT-Matrix" sheetId="3" r:id="rId2"/>
+    <sheet name="UniversityOtherOtherSets" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">UniversityOtherOtherSets!$A$1:$G$243</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">UniversityOtherOtherSets!$A$1:$G$243</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="31">
   <si>
     <t>input</t>
   </si>
@@ -85,49 +86,46 @@
     <t>otherOtherSets/Merged-5-set10-5.nt</t>
   </si>
   <si>
-    <t>Merged-1-2-3.nt</t>
+    <t>Univ-3</t>
   </si>
   <si>
-    <t>Merged-1-2.nt</t>
+    <t>Univ-4</t>
   </si>
   <si>
-    <t>Merged-2-3.nt</t>
+    <t>Univ-5</t>
   </si>
   <si>
-    <t>Merged-3-4-5.nt</t>
+    <t>Univ-1-2-3</t>
   </si>
   <si>
-    <t>Merged-3-4.nt</t>
+    <t>Univ-1-2</t>
   </si>
   <si>
-    <t>Merged-4-5.nt</t>
+    <t>Univ-2-3</t>
   </si>
   <si>
-    <t>Merged-5-set10-1.nt</t>
+    <t>Univ-3-4-5</t>
   </si>
   <si>
-    <t>Merged-5-set10-2.nt</t>
+    <t>Univ-3-4</t>
   </si>
   <si>
-    <t>Merged-5-set10-3.nt</t>
+    <t>Univ-4-5</t>
   </si>
   <si>
-    <t>Merged-5-set10-4.nt</t>
+    <t>Univ-1</t>
   </si>
   <si>
-    <t>Merged-5-set10-5.nt</t>
-  </si>
-  <si>
-    <t>Property Input/Other</t>
-  </si>
-  <si>
-    <t>PropertyAndType Input/Other</t>
+    <t>Univ-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -445,7 +443,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -560,6 +558,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -605,10 +618,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="10"/>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="10" xfId="10" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -932,930 +952,944 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="J6:L6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="B2" s="3">
+        <v>0.123291849749343</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.00061287507043</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.0009575287452801</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.0014652996012301</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.00237941839601</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.0089636547787899</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1.0066328281269901</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1.0075808117604199</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1.0168540844320499</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1.0111447279575401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.12983190894949401</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.99960164269533403</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.00002749317051</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.00125198562688</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.00442636101855</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.0045040134572201</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.0039396454006899</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.01177205569198</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1.0074855756077901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.00061287507043</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.12818385925578399</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.0009575287452801</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.0014652996012301</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.00237941839601</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.0089636547787899</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.0066328281269901</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1.0075808117604199</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1.0168540844320499</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.0111447279575401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="B5" s="2">
+        <v>1.002695281998</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.00448320558375</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0019474166531199</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.12711785310618301</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.00090790366017</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.00355999631487</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.0045580104780101</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.0045040134572201</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.0038622470565799</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.01177205569198</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1.0074855756077901</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="B6" s="2">
+        <v>1.002695281998</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.00448320558375</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.0019474166531199</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.13194407153027299</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.00288201213749</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.00143902263199</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1.00164474575381</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1.0015697621170701</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1.0039025205535199</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1.0031734235160501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="B7" s="2">
+        <v>1.0000500340326299</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.00005640994995</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.0000554055022199</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.999679558241101</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.99966543074348602</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.13177775195149999</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.0020051607146001</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.0018924752896401</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.0016692669820999</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1.00615596592629</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1.0031411061033699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="B8" s="2">
+        <v>1.07882294095733</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.0378382909633199</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.0423244784017001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.0638783585919001</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.02684030725145</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.0388990552086399</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.13746740358297599</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.0002620893188501</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.0000773813586901</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.00010357503258</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1.00032632650391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B9" s="2">
+        <v>1.0789771410217699</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.0380018624441401</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.04248598923115</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.0638783585919001</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.02684030725145</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.0386899578436499</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.99985929973530596</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.13565411185714599</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.0000773813586901</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1.00010357503258</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1.00009501153886</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2">
+      <c r="B10" s="2">
+        <v>1.0789771410217699</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.0380018624441401</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.04248598923115</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.0637977633101601</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.0267643607581001</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.03910815332044</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.00073961725423</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.0004458604245099</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.135411621039118</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1.00010357503258</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1.0005576424209801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.07887381099586</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.0378951228186299</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.0423803404585299</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.06395627413766</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.0269321832920799</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.0390026617705099</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.00062106944744</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1.00055131161921</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1.0001812064015301</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.14003435640943801</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1.0004626289765901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.07887381099586</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.0378951228186299</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.0423803404585299</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.06395627413766</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.0269321832920799</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1.03858446778592</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.99974075192853795</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1.0001837699737901</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1.0001812064015301</v>
+      </c>
+      <c r="K12" s="2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1.00061287507043</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1.0009575287452801</v>
-      </c>
-      <c r="F2">
-        <v>1.0014652996012301</v>
-      </c>
-      <c r="G2">
-        <v>1.00237941839601</v>
-      </c>
-      <c r="H2">
-        <v>1.0089636547787899</v>
-      </c>
-      <c r="I2">
-        <v>1.0066328281269901</v>
-      </c>
-      <c r="J2">
-        <v>1.0075808117604199</v>
-      </c>
-      <c r="K2">
-        <v>1.0168540844320499</v>
-      </c>
-      <c r="L2">
-        <v>1.0111447279575401</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0.99960164269533403</v>
-      </c>
-      <c r="F3">
-        <v>1.00002749317051</v>
-      </c>
-      <c r="G3">
-        <v>1.00125198562688</v>
-      </c>
-      <c r="H3">
-        <v>1.00442636101855</v>
-      </c>
-      <c r="I3">
-        <v>1.0045040134572201</v>
-      </c>
-      <c r="J3">
-        <v>1.0039396454006899</v>
-      </c>
-      <c r="K3">
-        <v>1.01177205569198</v>
-      </c>
-      <c r="L3">
-        <v>1.0074855756077901</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1.00061287507043</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1.0009575287452801</v>
-      </c>
-      <c r="F4">
-        <v>1.0014652996012301</v>
-      </c>
-      <c r="G4">
-        <v>1.00237941839601</v>
-      </c>
-      <c r="H4">
-        <v>1.0089636547787899</v>
-      </c>
-      <c r="I4">
-        <v>1.0066328281269901</v>
-      </c>
-      <c r="J4">
-        <v>1.0075808117604199</v>
-      </c>
-      <c r="K4">
-        <v>1.0168540844320499</v>
-      </c>
-      <c r="L4">
-        <v>1.0111447279575401</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5">
-        <v>1.002695281998</v>
-      </c>
-      <c r="C5">
-        <v>1.00448320558375</v>
-      </c>
-      <c r="D5">
-        <v>1.0019474166531199</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1.00090790366017</v>
-      </c>
-      <c r="G5">
-        <v>1.00355999631487</v>
-      </c>
-      <c r="H5">
-        <v>1.0045580104780101</v>
-      </c>
-      <c r="I5">
-        <v>1.0045040134572201</v>
-      </c>
-      <c r="J5">
-        <v>1.0038622470565799</v>
-      </c>
-      <c r="K5">
-        <v>1.01177205569198</v>
-      </c>
-      <c r="L5">
-        <v>1.0074855756077901</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6">
-        <v>1.002695281998</v>
-      </c>
-      <c r="C6">
-        <v>1.00448320558375</v>
-      </c>
-      <c r="D6">
-        <v>1.0019474166531199</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1.00288201213749</v>
-      </c>
-      <c r="H6">
-        <v>1.00143902263199</v>
-      </c>
-      <c r="I6">
-        <v>1.00164474575381</v>
-      </c>
-      <c r="J6">
-        <v>1.0015697621170701</v>
-      </c>
-      <c r="K6">
-        <v>1.0039025205535199</v>
-      </c>
-      <c r="L6">
-        <v>1.0031734235160501</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7">
-        <v>1.0000500340326299</v>
-      </c>
-      <c r="C7">
-        <v>1.00005640994995</v>
-      </c>
-      <c r="D7">
-        <v>1.0000554055022199</v>
-      </c>
-      <c r="E7">
-        <v>0.999679558241101</v>
-      </c>
-      <c r="F7">
-        <v>0.99966543074348602</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1.0020051607146001</v>
-      </c>
-      <c r="I7">
-        <v>1.0018924752896401</v>
-      </c>
-      <c r="J7">
-        <v>1.0016692669820999</v>
-      </c>
-      <c r="K7">
-        <v>1.00615596592629</v>
-      </c>
-      <c r="L7">
-        <v>1.0031411061033699</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8">
-        <v>1.07882294095733</v>
-      </c>
-      <c r="C8">
-        <v>1.0378382909633199</v>
-      </c>
-      <c r="D8">
-        <v>1.0423244784017001</v>
-      </c>
-      <c r="E8">
-        <v>1.0638783585919001</v>
-      </c>
-      <c r="F8">
-        <v>1.02684030725145</v>
-      </c>
-      <c r="G8">
-        <v>1.0388990552086399</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1.0002620893188501</v>
-      </c>
-      <c r="J8">
-        <v>1.0000773813586901</v>
-      </c>
-      <c r="K8">
-        <v>1.00010357503258</v>
-      </c>
-      <c r="L8">
-        <v>1.00032632650391</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9">
-        <v>1.0789771410217699</v>
-      </c>
-      <c r="C9">
-        <v>1.0380018624441401</v>
-      </c>
-      <c r="D9">
-        <v>1.04248598923115</v>
-      </c>
-      <c r="E9">
-        <v>1.0638783585919001</v>
-      </c>
-      <c r="F9">
-        <v>1.02684030725145</v>
-      </c>
-      <c r="G9">
-        <v>1.0386899578436499</v>
-      </c>
-      <c r="H9">
-        <v>0.99985929973530596</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1.0000773813586901</v>
-      </c>
-      <c r="K9">
-        <v>1.00010357503258</v>
-      </c>
-      <c r="L9">
-        <v>1.00009501153886</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10">
-        <v>1.0789771410217699</v>
-      </c>
-      <c r="C10">
-        <v>1.0380018624441401</v>
-      </c>
-      <c r="D10">
-        <v>1.04248598923115</v>
-      </c>
-      <c r="E10">
-        <v>1.0637977633101601</v>
-      </c>
-      <c r="F10">
-        <v>1.0267643607581001</v>
-      </c>
-      <c r="G10">
-        <v>1.03910815332044</v>
-      </c>
-      <c r="H10">
-        <v>1.00073961725423</v>
-      </c>
-      <c r="I10">
-        <v>1.0004458604245099</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1.00010357503258</v>
-      </c>
-      <c r="L10">
-        <v>1.0005576424209801</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11">
-        <v>1.07887381099586</v>
-      </c>
-      <c r="C11">
-        <v>1.0378951228186299</v>
-      </c>
-      <c r="D11">
-        <v>1.0423803404585299</v>
-      </c>
-      <c r="E11">
-        <v>1.06395627413766</v>
-      </c>
-      <c r="F11">
-        <v>1.0269321832920799</v>
-      </c>
-      <c r="G11">
-        <v>1.0390026617705099</v>
-      </c>
-      <c r="H11">
-        <v>1.00062106944744</v>
-      </c>
-      <c r="I11">
-        <v>1.00055131161921</v>
-      </c>
-      <c r="J11">
-        <v>1.0001812064015301</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1.0004626289765901</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12">
-        <v>1.07887381099586</v>
-      </c>
-      <c r="C12">
-        <v>1.0378951228186299</v>
-      </c>
-      <c r="D12">
-        <v>1.0423803404585299</v>
-      </c>
-      <c r="E12">
-        <v>1.06395627413766</v>
-      </c>
-      <c r="F12">
-        <v>1.0269321832920799</v>
-      </c>
-      <c r="G12">
-        <v>1.03858446778592</v>
-      </c>
-      <c r="H12">
-        <v>0.99974075192853795</v>
-      </c>
-      <c r="I12">
-        <v>1.0001837699737901</v>
-      </c>
-      <c r="J12">
-        <v>1.0001812064015301</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
+      <c r="L12" s="3">
+        <v>0.13716878865755699</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="K14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="L14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="B15" s="3">
+        <v>0.11167679798833199</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.0360744555235</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.0286951188765401</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.0351467012339</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.05121355067884</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.0490620538834601</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.09804194470534</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1.09365261856186</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.0934282451658699</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.11947471834668</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1.1008980168031499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="B16" s="2">
+        <v>1.04973975153058</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.120777529059479</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.0252750657621399</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.04797390145064</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.0278395781751799</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.02581747843028</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.0505273189028099</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1.04634568974432</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1.04899160492934</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.0680395392340301</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1.0569401274110199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="B17" s="2">
+        <v>1.0554437861611199</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.0332314765244499</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.11887838900044299</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1.0548710425711401</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.0339134851187299</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.0335742366705001</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.06693713219538</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1.06136623562029</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1.05988865948014</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.0860393574752301</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1.0675401241700599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="B18" s="2">
+        <v>1.02891099124005</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.0298886378348799</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1.0264273768418599</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.117238090994866</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1.02552750690862</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1.02778354324883</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1.0583166417296399</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1.05370952178124</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1.05287983579277</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1.0751770717231901</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1.06179732505352</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="B19" s="2">
+        <v>1.06931669522164</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.02981984266701</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1.02711117395928</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.0480863400443701</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.12349039010286</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1.02410354696997</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1.0350839536018901</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1.03376528710473</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1.02945603268102</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1.04717311600745</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1.03654059145623</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="B20" s="2">
+        <v>1.07232969163725</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1.0327612805816799</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.0312337851829101</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.05601351365244</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1.0305633535890599</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.123010817005099</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1.04721023861047</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1.04553456522121</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1.04282438993945</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1.0583070617027299</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1.04273719162763</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="B21" s="2">
+        <v>1.2438877652350799</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1.1377278494605201</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1.1524912438222199</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1.1929611844257599</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1.10522394203393</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1.12039308877892</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.125840231482688</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1.02655044916551</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1.0225076155893</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1.0224738189843701</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1.0193198897983</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B22" s="2">
+        <v>1.2499475020761199</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.1361016910956401</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1.15040266864082</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.19831652816992</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1.1057662083905799</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1.12228937251873</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1.0232848874629901</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.124039801239966</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1.02424603265868</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1.0241202331680099</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1.0185824640374099</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1.0360744555235</v>
-      </c>
-      <c r="D15">
-        <v>1.0286951188765401</v>
-      </c>
-      <c r="E15">
-        <v>1.0351467012339</v>
-      </c>
-      <c r="F15">
-        <v>1.05121355067884</v>
-      </c>
-      <c r="G15">
-        <v>1.0490620538834601</v>
-      </c>
-      <c r="H15">
-        <v>1.09804194470534</v>
-      </c>
-      <c r="I15">
-        <v>1.09365261856186</v>
-      </c>
-      <c r="J15">
-        <v>1.0934282451658699</v>
-      </c>
-      <c r="K15">
-        <v>1.11947471834668</v>
-      </c>
-      <c r="L15">
-        <v>1.1008980168031499</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="B23" s="2">
+        <v>1.2398786491090099</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.1344620969621499</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.1448602763395901</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1.18724926399349</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.0976537684632199</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1.11758907254323</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1.0206532173524501</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1.02390905750337</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0.123836578098501</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1.02241440787968</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1.0171267141984199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
-        <v>1.04973975153058</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1.0252750657621399</v>
-      </c>
-      <c r="E16">
-        <v>1.04797390145064</v>
-      </c>
-      <c r="F16">
-        <v>1.0278395781751799</v>
-      </c>
-      <c r="G16">
-        <v>1.02581747843028</v>
-      </c>
-      <c r="H16">
-        <v>1.0505273189028099</v>
-      </c>
-      <c r="I16">
-        <v>1.04634568974432</v>
-      </c>
-      <c r="J16">
-        <v>1.04899160492934</v>
-      </c>
-      <c r="K16">
-        <v>1.0680395392340301</v>
-      </c>
-      <c r="L16">
-        <v>1.0569401274110199</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B24" s="2">
+        <v>1.2695488519159099</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.1563158665623401</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1.1705476796832599</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.21423220279646</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.11798599150593</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1.1340174901853599</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1.0258326674362701</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1.0297888817741601</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1.0280904556191199</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0.12764222327813099</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1.0219355963749801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17">
-        <v>1.0554437861611199</v>
-      </c>
-      <c r="C17">
-        <v>1.0332314765244499</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1.0548710425711401</v>
-      </c>
-      <c r="F17">
-        <v>1.0339134851187299</v>
-      </c>
-      <c r="G17">
-        <v>1.0335742366705001</v>
-      </c>
-      <c r="H17">
-        <v>1.06693713219538</v>
-      </c>
-      <c r="I17">
-        <v>1.06136623562029</v>
-      </c>
-      <c r="J17">
-        <v>1.05988865948014</v>
-      </c>
-      <c r="K17">
-        <v>1.0860393574752301</v>
-      </c>
-      <c r="L17">
-        <v>1.0675401241700599</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <v>1.02891099124005</v>
-      </c>
-      <c r="C18">
-        <v>1.0298886378348799</v>
-      </c>
-      <c r="D18">
-        <v>1.0264273768418599</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1.02552750690862</v>
-      </c>
-      <c r="G18">
-        <v>1.02778354324883</v>
-      </c>
-      <c r="H18">
-        <v>1.0583166417296399</v>
-      </c>
-      <c r="I18">
-        <v>1.05370952178124</v>
-      </c>
-      <c r="J18">
-        <v>1.05287983579277</v>
-      </c>
-      <c r="K18">
-        <v>1.0751770717231901</v>
-      </c>
-      <c r="L18">
-        <v>1.06179732505352</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>1.06931669522164</v>
-      </c>
-      <c r="C19">
-        <v>1.02981984266701</v>
-      </c>
-      <c r="D19">
-        <v>1.02711117395928</v>
-      </c>
-      <c r="E19">
-        <v>1.0480863400443701</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>1.02410354696997</v>
-      </c>
-      <c r="H19">
-        <v>1.0350839536018901</v>
-      </c>
-      <c r="I19">
-        <v>1.03376528710473</v>
-      </c>
-      <c r="J19">
-        <v>1.02945603268102</v>
-      </c>
-      <c r="K19">
-        <v>1.04717311600745</v>
-      </c>
-      <c r="L19">
-        <v>1.03654059145623</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <v>1.07232969163725</v>
-      </c>
-      <c r="C20">
-        <v>1.0327612805816799</v>
-      </c>
-      <c r="D20">
-        <v>1.0312337851829101</v>
-      </c>
-      <c r="E20">
-        <v>1.05601351365244</v>
-      </c>
-      <c r="F20">
-        <v>1.0305633535890599</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>1.04721023861047</v>
-      </c>
-      <c r="I20">
-        <v>1.04553456522121</v>
-      </c>
-      <c r="J20">
-        <v>1.04282438993945</v>
-      </c>
-      <c r="K20">
-        <v>1.0583070617027299</v>
-      </c>
-      <c r="L20">
-        <v>1.04273719162763</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
-        <v>1.2438877652350799</v>
-      </c>
-      <c r="C21">
-        <v>1.1377278494605201</v>
-      </c>
-      <c r="D21">
-        <v>1.1524912438222199</v>
-      </c>
-      <c r="E21">
-        <v>1.1929611844257599</v>
-      </c>
-      <c r="F21">
-        <v>1.10522394203393</v>
-      </c>
-      <c r="G21">
-        <v>1.12039308877892</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>1.02655044916551</v>
-      </c>
-      <c r="J21">
-        <v>1.0225076155893</v>
-      </c>
-      <c r="K21">
-        <v>1.0224738189843701</v>
-      </c>
-      <c r="L21">
-        <v>1.0193198897983</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22">
-        <v>1.2499475020761199</v>
-      </c>
-      <c r="C22">
-        <v>1.1361016910956401</v>
-      </c>
-      <c r="D22">
-        <v>1.15040266864082</v>
-      </c>
-      <c r="E22">
-        <v>1.19831652816992</v>
-      </c>
-      <c r="F22">
-        <v>1.1057662083905799</v>
-      </c>
-      <c r="G22">
-        <v>1.12228937251873</v>
-      </c>
-      <c r="H22">
-        <v>1.0232848874629901</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>1.02424603265868</v>
-      </c>
-      <c r="K22">
-        <v>1.0241202331680099</v>
-      </c>
-      <c r="L22">
-        <v>1.0185824640374099</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23">
-        <v>1.2398786491090099</v>
-      </c>
-      <c r="C23">
-        <v>1.1344620969621499</v>
-      </c>
-      <c r="D23">
-        <v>1.1448602763395901</v>
-      </c>
-      <c r="E23">
-        <v>1.18724926399349</v>
-      </c>
-      <c r="F23">
-        <v>1.0976537684632199</v>
-      </c>
-      <c r="G23">
-        <v>1.11758907254323</v>
-      </c>
-      <c r="H23">
-        <v>1.0206532173524501</v>
-      </c>
-      <c r="I23">
-        <v>1.02390905750337</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23">
-        <v>1.02241440787968</v>
-      </c>
-      <c r="L23">
-        <v>1.0171267141984199</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24">
-        <v>1.2695488519159099</v>
-      </c>
-      <c r="C24">
-        <v>1.1563158665623401</v>
-      </c>
-      <c r="D24">
-        <v>1.1705476796832599</v>
-      </c>
-      <c r="E24">
-        <v>1.21423220279646</v>
-      </c>
-      <c r="F24">
-        <v>1.11798599150593</v>
-      </c>
-      <c r="G24">
-        <v>1.1340174901853599</v>
-      </c>
-      <c r="H24">
-        <v>1.0258326674362701</v>
-      </c>
-      <c r="I24">
-        <v>1.0297888817741601</v>
-      </c>
-      <c r="J24">
-        <v>1.0280904556191199</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>1.0219355963749801</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>1.2627402764771201</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>1.1493689897704</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>1.16105685316814</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>1.20440262321063</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>1.1114982367633</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>1.1244722854354099</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="2">
         <v>1.0224006326684101</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="2">
         <v>1.0249393870887</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="2">
         <v>1.0227515264140301</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="2">
         <v>1.0245660747038401</v>
       </c>
-      <c r="L25">
-        <v>1</v>
+      <c r="L25" s="3">
+        <v>0.12538062381413201</v>
       </c>
     </row>
   </sheetData>
@@ -1863,7 +1897,9 @@
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
+        <cfvo type="num" val="1"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
@@ -1873,7 +1909,969 @@
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
+        <cfvo type="num" val="1"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.123291849749343</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.00088891374293</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.0011994102166399</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.0019933756904</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.0032508651094001</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.0093163424296201</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1.0071750501145</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1.0077678776840799</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1.01710731072048</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1.0118009495506499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.12983190894949401</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.99960302970423498</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.0003010600816</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.0017895870878499</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.0045265985149701</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.00478065230228</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.0038875021440401</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.01167120131917</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1.0078301554675899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.00088891374293</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.12818385925578399</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.0011994102166399</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.0019933756904</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.0032508651094001</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.0093163424296201</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.0071750501145</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1.0077678776840799</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1.01710731072048</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.0118009495506499</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.00282385764791</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.00461701882315</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0020869597200099</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.12711785310618301</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.00117854374288</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.00408534049404</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.00465677962348</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.00478065230228</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1.00381033862403</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1.01167120131917</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1.0078301554675899</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.00282385764791</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.00461701882315</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.0020869597200099</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.13194407153027299</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.0034353189054801</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.0019339991181599</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1.0021079142945299</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1.0016925784982</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1.0040631710061401</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1.0037357387865</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.00004993534738</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.00005628607609</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.0000552905729301</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.99982464511848501</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.99995599328562501</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.13177775195149999</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.0019868211118801</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.0018680729552201</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.00181504300376</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1.0060986942282999</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1.00310649272745</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.0785856476546001</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.0376682800753401</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.0421412247488899</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.0636404205205701</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.02666851286937</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.0388498037107901</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.13746740358297599</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.0004284112425701</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1.0000771465915099</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.00010316307909</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1.0005348553598801</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.0788801383975499</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.03798047669612</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.0424495613123299</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.0636404205205701</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.02666851286937</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.03845161155448</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.00006048834022</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.13565411185714599</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.0000771465915099</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1.00010316307909</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1.0000946464226701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.0788801383975499</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.03798047669612</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.0424495613123299</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.0635601076608701</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.0265927981465801</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.0392479980989999</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.0010801985295299</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.0007787587641599</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.135411621039118</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1.00010316307909</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1.0009750671445099</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.0786364164797699</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.03772498642059</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.0421969702389999</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.06386272325302</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.02691300514831</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.03914301579152</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.00078076487301</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1.00105103917893</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1.00034555311428</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.14003435640943801</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1.0008804169252801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.0786364164797699</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.03772498642059</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.0421969702389999</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.06386272325302</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.02691300514831</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1.0383466322211601</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.99976105811773597</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1.0003503446995901</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1.00034555311428</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.13716878865755699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.11167679798833199</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.0312054109075901</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.0262879565163801</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.03236850382157</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.04355062210771</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.04190008107351</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.0810988482192601</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1.0772891074723701</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.0780649245429701</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.0959674590319901</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1.08446101645107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.04387799231258</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.120777529059479</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.02280858120061</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.04238192021525</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.0248002253680499</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.02331908461085</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.0417725188517299</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1.0374820829412901</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1.0395713007819101</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.0540950820670301</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1.0476812817712799</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.04964145846303</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.0294523531326101</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.11887838900044299</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1.05040725771985</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.02985358023943</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.03200950847063</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.0556043689764001</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1.05110519232483</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1.0503036494304401</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.06960397608027</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1.0571876244907099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.0263325619113099</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.0267872270945799</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1.0243917004691501</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.117238090994866</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1.0230737522472799</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1.02657848248324</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1.04558808664752</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1.04225849141994</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1.04226777005753</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1.05729103231057</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1.0503251974335399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.06027275788802</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.0246097530834399</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1.0227550695763801</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.0409390517966499</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.12349039010286</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1.0240202787910799</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1.0289693203236201</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1.0279475137708201</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1.0252083812833599</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1.03717131809859</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1.0314264166254601</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.0609794625259401</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1.0254334611212199</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.0248827043755599</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.04656842978298</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1.02465338343139</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.123010817005099</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1.0391766098152999</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1.0367504901648901</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1.03569594073795</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1.0469027867105001</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1.0360493283252199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1.24670063236143</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1.13529252586517</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1.1516778568878501</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1.1934638141158</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1.1026612031920899</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1.12223712527674</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.125840231482688</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1.0201534361406599</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1.0167433352266</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1.01643537774293</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1.01547762338942</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.25468713783301</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.13605494878229</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1.1520128279978199</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.2002265644685599</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1.1045561510864901</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1.1260278814708999</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1.0185164744633699</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.124039801239966</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1.01878814150025</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1.01903259172373</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1.01593533725577</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1.24429182903728</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.1325734685826401</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.14564314416298</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1.18865707430422</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.09700373941706</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1.1207315504233799</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1.0173518186895301</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1.0174699271660399</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.123836578098501</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1.0175696789233699</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1.01458817246868</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.2702860219352401</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.1501668895066199</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1.1661855537222601</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.2114241020497201</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.11205496447324</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1.1320824446120701</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1.01809981451469</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1.02028487783059</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1.01940198813372</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.12764222327813099</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1.01633731623914</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1.26425898001597</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1.14469821422885</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1.15807370657797</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1.2027573383807799</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1.1066275066483899</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1.1251254972672999</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1.0156227547024901</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1.01676470958897</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1.0153811137694899</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1.0178446438878901</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.12538062381413201</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:L12">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:L25">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
@@ -1883,18 +2881,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G243"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G223" sqref="G223:G243"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E242" sqref="E242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -6980,7 +7979,7 @@
         <v>1.0219355963749801</v>
       </c>
     </row>
-    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>19</v>
       </c>
@@ -7003,7 +8002,7 @@
         <v>1.07887381099586</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>19</v>
       </c>
@@ -7026,7 +8025,7 @@
         <v>1.2627402764771201</v>
       </c>
     </row>
-    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>19</v>
       </c>
@@ -7049,7 +8048,7 @@
         <v>1.0378951228186299</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>19</v>
       </c>
@@ -7072,7 +8071,7 @@
         <v>1.1493689897704</v>
       </c>
     </row>
-    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>19</v>
       </c>
@@ -7095,7 +8094,7 @@
         <v>1.0423803404585299</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>19</v>
       </c>
@@ -7118,7 +8117,7 @@
         <v>1.16105685316814</v>
       </c>
     </row>
-    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>19</v>
       </c>
@@ -7141,7 +8140,7 @@
         <v>1.06395627413766</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>19</v>
       </c>
@@ -7164,7 +8163,7 @@
         <v>1.20440262321063</v>
       </c>
     </row>
-    <row r="230" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>19</v>
       </c>
@@ -7187,7 +8186,7 @@
         <v>1.0269321832920799</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>19</v>
       </c>
@@ -7210,7 +8209,7 @@
         <v>1.1114982367633</v>
       </c>
     </row>
-    <row r="232" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>19</v>
       </c>
@@ -7233,7 +8232,7 @@
         <v>1.03858446778592</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>19</v>
       </c>
@@ -7256,7 +8255,7 @@
         <v>1.1244722854354099</v>
       </c>
     </row>
-    <row r="234" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>19</v>
       </c>
@@ -7279,7 +8278,7 @@
         <v>0.99974075192853795</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>19</v>
       </c>
@@ -7302,7 +8301,7 @@
         <v>1.0224006326684101</v>
       </c>
     </row>
-    <row r="236" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>19</v>
       </c>
@@ -7325,7 +8324,7 @@
         <v>1.0001837699737901</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>19</v>
       </c>
@@ -7348,7 +8347,7 @@
         <v>1.0249393870887</v>
       </c>
     </row>
-    <row r="238" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>19</v>
       </c>
@@ -7371,7 +8370,7 @@
         <v>1.0001812064015301</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>19</v>
       </c>
@@ -7394,7 +8393,7 @@
         <v>1.0227515264140301</v>
       </c>
     </row>
-    <row r="240" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>19</v>
       </c>
@@ -7417,7 +8416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>19</v>
       </c>
@@ -7440,7 +8439,7 @@
         <v>1.0245660747038401</v>
       </c>
     </row>
-    <row r="242" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>19</v>
       </c>
@@ -7463,7 +8462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>19</v>
       </c>
@@ -7495,7 +8494,7 @@
     </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="PropertyAndType"/>
+        <filter val="Property"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>